<commit_message>
Criando teste de cadastro no cucumber.
</commit_message>
<xml_diff>
--- a/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
+++ b/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\jee\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB3483A-1DE6-4F45-891D-E271EF6E0A0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F0D1C63E-1E31-4ECE-AA52-7E35E332E56D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="1635" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15405" windowHeight="11340" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -19,6 +14,7 @@
     <sheet name="Pagamento" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:C4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -314,13 +310,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -640,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B732072B-4DFA-4889-A7A4-3C1058C30EFF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,16 +657,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -692,7 +688,7 @@
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
@@ -871,15 +867,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -923,10 +919,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1"/>
       <c r="D5" s="4" t="s">
         <v>49</v>
@@ -954,10 +950,10 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -989,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BBC43E-FC47-4208-85C2-FA45BE08B035}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C7" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1003,15 +999,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1049,10 +1045,10 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1091,10 +1087,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Cenarios de sucesso e falha de cadastro criados.
</commit_message>
<xml_diff>
--- a/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
+++ b/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F0D1C63E-1E31-4ECE-AA52-7E35E332E56D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\git\projeto-bdd\projeto-bdd\main\br\com\rsinet\hub_bdd\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95A9B59-FA77-4CBB-9D3F-85099CD449A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15405" windowHeight="11340" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,6 @@
     <sheet name="Pagamento" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:C4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -209,13 +213,13 @@
     <t>EscolheProduto</t>
   </si>
   <si>
-    <t>lucascarvalh9</t>
-  </si>
-  <si>
     <t>HP Z3600 Wireless Mouse</t>
   </si>
   <si>
     <t>HP Z3600 WIRELESS MOUSE</t>
+  </si>
+  <si>
+    <t>lucascarval14</t>
   </si>
 </sst>
 </file>
@@ -636,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B732072B-4DFA-4889-A7A4-3C1058C30EFF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +677,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1021,7 +1025,7 @@
         <v>58</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,7 +1033,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4" t="s">

</xml_diff>

<commit_message>
Cenario de pesquisa por categoria criado.
</commit_message>
<xml_diff>
--- a/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
+++ b/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\git\projeto-bdd\projeto-bdd\main\br\com\rsinet\hub_bdd\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\jee\projeto-bdd\projeto-bdd\main\br\com\rsinet\hub_bdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95A9B59-FA77-4CBB-9D3F-85099CD449A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5815FBF7-98FD-473D-ADA6-5DBBA6D94541}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -219,7 +219,7 @@
     <t>HP Z3600 WIRELESS MOUSE</t>
   </si>
   <si>
-    <t>lucascarval14</t>
+    <t>lucascarval17</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Cenarios de consulta por barra de pesquisa criados.
</commit_message>
<xml_diff>
--- a/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
+++ b/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\jee\projeto-bdd\projeto-bdd\main\br\com\rsinet\hub_bdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5815FBF7-98FD-473D-ADA6-5DBBA6D94541}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C83FE0F-E4A3-457F-A5B4-DA362DD21ECB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -640,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B732072B-4DFA-4889-A7A4-3C1058C30EFF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BBC43E-FC47-4208-85C2-FA45BE08B035}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Codigos comentados para melhor entendimento.
</commit_message>
<xml_diff>
--- a/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
+++ b/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\jee\projeto-bdd\projeto-bdd\main\br\com\rsinet\hub_bdd\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\git\projeto-bdd\projeto-bdd\main\br\com\rsinet\hub_bdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C83FE0F-E4A3-457F-A5B4-DA362DD21ECB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6C717A-3DD4-4434-AB99-13C9DEB9BF29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -219,7 +219,7 @@
     <t>HP Z3600 WIRELESS MOUSE</t>
   </si>
   <si>
-    <t>lucascarval17</t>
+    <t>lucascarval23</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B732072B-4DFA-4889-A7A4-3C1058C30EFF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -989,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BBC43E-FC47-4208-85C2-FA45BE08B035}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajustando testes ao workspace da rsi.
</commit_message>
<xml_diff>
--- a/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
+++ b/projeto-bdd/main/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\git\projeto-bdd\projeto-bdd\main\br\com\rsinet\hub_bdd\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-bdd\projeto-bdd\main\br\com\rsinet\hub_bdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D527A419-1563-401F-BADB-8D16C3DC35C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B78A8D-D9BD-4F9F-BA5B-6774E951C302}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -216,10 +216,10 @@
     <t>HP Z3600 WIRELESS MOUSE</t>
   </si>
   <si>
-    <t>lucascarval36</t>
-  </si>
-  <si>
     <t>HP Z3600 Wireless Mouse</t>
+  </si>
+  <si>
+    <t>lucascarval40</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B732072B-4DFA-4889-A7A4-3C1058C30EFF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -677,7 +677,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -989,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BBC43E-FC47-4208-85C2-FA45BE08B035}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1033,7 +1033,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4" t="s">

</xml_diff>